<commit_message>
All RL results are now in
</commit_message>
<xml_diff>
--- a/pyFiles/RL/Results/New Results/PPJ.xlsx
+++ b/pyFiles/RL/Results/New Results/PPJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bozho1\Desktop\Thesis Code\ThesisWorkCybercom\pyFiles\RL\Results\New Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D80D50F-323C-4039-A4CA-FC5C9EB62C43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B80A65-0250-4B09-8329-8AAB7137FED2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{73710C65-8F07-465A-A6D4-9129311F8791}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>PPJ Results</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 29363000]</t>
+  </si>
+  <si>
+    <t>Fix Node Placement</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533BF79D-71AF-4EDC-83CB-C796A49BE4BB}">
-  <dimension ref="A1:QF45"/>
+  <dimension ref="A1:QF48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18563,8 +18566,13 @@
         <v>24</v>
       </c>
     </row>
+    <row r="48" spans="1:375" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A48" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>